<commit_message>
Fixed n on leaf size graphs
</commit_message>
<xml_diff>
--- a/Prototypes/Barley/LeafSizeObserved.xlsx
+++ b/Prototypes/Barley/LeafSizeObserved.xlsx
@@ -29,12 +29,6 @@
     <t>SimulationName</t>
   </si>
   <si>
-    <t>LeafSize.Script.LeafExpandedPosition</t>
-  </si>
-  <si>
-    <t>LeafSize.Script.MostRecentlyExpandedLeafSize</t>
-  </si>
-  <si>
     <t>MCPD11_12CultBoomaSD1</t>
   </si>
   <si>
@@ -63,6 +57,12 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>MaxLeafSize.Script.LeafPosition</t>
+  </si>
+  <si>
+    <t>MaxLeafSize.Script.MaxLeafSize</t>
   </si>
 </sst>
 </file>
@@ -384,12 +384,13 @@
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D103"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -397,18 +398,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -422,7 +423,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -436,7 +437,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -450,7 +451,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -464,7 +465,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -478,7 +479,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -492,7 +493,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -506,7 +507,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -520,7 +521,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -534,7 +535,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -548,7 +549,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -562,7 +563,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -576,7 +577,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -590,7 +591,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -604,7 +605,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -618,7 +619,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -632,7 +633,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -646,7 +647,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19">
         <v>7</v>
@@ -660,7 +661,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -674,7 +675,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <v>9</v>
@@ -688,7 +689,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -702,7 +703,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23">
         <v>11</v>
@@ -716,7 +717,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24">
         <v>12</v>
@@ -728,7 +729,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -742,7 +743,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -756,7 +757,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -770,7 +771,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -784,7 +785,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B29">
         <v>5</v>
@@ -798,7 +799,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B30">
         <v>6</v>
@@ -812,7 +813,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B31">
         <v>7</v>
@@ -826,7 +827,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -840,7 +841,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B33">
         <v>9</v>
@@ -854,7 +855,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -868,7 +869,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B35">
         <v>11</v>
@@ -880,7 +881,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -894,7 +895,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -908,7 +909,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -922,7 +923,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -936,7 +937,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B40">
         <v>5</v>
@@ -950,7 +951,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B41">
         <v>6</v>
@@ -964,7 +965,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B42">
         <v>7</v>
@@ -978,7 +979,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -992,7 +993,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B44">
         <v>9</v>
@@ -1006,7 +1007,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B45">
         <v>10</v>
@@ -1020,7 +1021,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B46">
         <v>11</v>
@@ -1034,7 +1035,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1048,7 +1049,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -1062,7 +1063,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -1076,7 +1077,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B50">
         <v>4</v>
@@ -1090,7 +1091,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B51">
         <v>5</v>
@@ -1104,7 +1105,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -1118,7 +1119,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B53">
         <v>7</v>
@@ -1132,7 +1133,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B54">
         <v>8</v>
@@ -1146,7 +1147,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B55">
         <v>9</v>
@@ -1160,7 +1161,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B56">
         <v>10</v>
@@ -1174,7 +1175,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B57">
         <v>11</v>
@@ -1188,7 +1189,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B58">
         <v>12</v>
@@ -1200,7 +1201,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1214,7 +1215,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -1228,7 +1229,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B61">
         <v>3</v>
@@ -1242,7 +1243,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -1256,7 +1257,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B63">
         <v>5</v>
@@ -1270,7 +1271,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B64">
         <v>6</v>
@@ -1284,7 +1285,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B65">
         <v>7</v>
@@ -1298,7 +1299,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -1312,7 +1313,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B67">
         <v>9</v>
@@ -1326,7 +1327,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B68">
         <v>10</v>
@@ -1340,7 +1341,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B69">
         <v>11</v>
@@ -1354,7 +1355,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -1368,7 +1369,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -1382,7 +1383,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B72">
         <v>3</v>
@@ -1396,7 +1397,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B73">
         <v>4</v>
@@ -1410,7 +1411,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B74">
         <v>5</v>
@@ -1424,7 +1425,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B75">
         <v>6</v>
@@ -1438,7 +1439,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B76">
         <v>7</v>
@@ -1452,7 +1453,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B77">
         <v>8</v>
@@ -1466,7 +1467,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B78">
         <v>9</v>
@@ -1480,7 +1481,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B79">
         <v>10</v>
@@ -1494,7 +1495,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B80">
         <v>11</v>
@@ -1508,7 +1509,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -1522,7 +1523,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B82">
         <v>2</v>
@@ -1536,7 +1537,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -1550,7 +1551,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B84">
         <v>4</v>
@@ -1564,7 +1565,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B85">
         <v>5</v>
@@ -1578,7 +1579,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B86">
         <v>6</v>
@@ -1592,7 +1593,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B87">
         <v>7</v>
@@ -1606,7 +1607,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B88">
         <v>8</v>
@@ -1620,7 +1621,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B89">
         <v>9</v>
@@ -1634,7 +1635,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B90">
         <v>10</v>
@@ -1648,7 +1649,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B91">
         <v>11</v>
@@ -1660,7 +1661,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B92">
         <v>12</v>
@@ -1672,7 +1673,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -1686,7 +1687,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -1700,7 +1701,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -1714,7 +1715,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B96">
         <v>4</v>
@@ -1728,7 +1729,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B97">
         <v>5</v>
@@ -1742,7 +1743,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B98">
         <v>6</v>
@@ -1756,7 +1757,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B99">
         <v>7</v>
@@ -1770,7 +1771,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B100">
         <v>8</v>
@@ -1784,7 +1785,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B101">
         <v>9</v>
@@ -1798,7 +1799,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B102">
         <v>10</v>
@@ -1810,7 +1811,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B103">
         <v>11</v>

</xml_diff>